<commit_message>
Bugs for multiport processing fixed
</commit_message>
<xml_diff>
--- a/DoSDetector/models/model_stats.xlsx
+++ b/DoSDetector/models/model_stats.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -757,6 +757,40 @@
         <v>0.007092167696623517</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>AdaBoostClassifier</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.9947049924357034</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.9947424529098876</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.9947026872498572</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9947039454146909</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.4025695323944092</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.01609516143798828</v>
+      </c>
+      <c r="H10" t="n">
+        <v>1.217485736610309e-05</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.9927355278093076</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.005448354143019296</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>